<commit_message>
resolve test suite conflict
</commit_message>
<xml_diff>
--- a/Excel Files/Scenario 9/S9_TestCases_Data.xlsx
+++ b/Excel Files/Scenario 9/S9_TestCases_Data.xlsx
@@ -1,79 +1,79 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huawe\git\tb-ttap-brivge-fatin\Excel Files\Scenario 9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huawe\git\tb-ttap-brivge-v2-fatin\Excel Files\Scenario 9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{CB8DF930-A083-4BE3-8A62-3EBC010CA90E}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A0BF1F-D43E-4722-93FC-2D8397498B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="54" firstSheet="50" windowHeight="15840" windowWidth="29040" xWindow="28680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="31" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TC1-Request Add New" r:id="rId1" sheetId="1"/>
-    <sheet name="TC1" r:id="rId2" sheetId="3"/>
-    <sheet name="TC1.1&amp;3.1-Payment Terms" r:id="rId3" sheetId="4"/>
-    <sheet name="TC1.2-BU ShippingRoute" r:id="rId4" sheetId="5"/>
-    <sheet name="TC1.2-ETAnWeek" r:id="rId5" sheetId="6"/>
-    <sheet name="TC2-Contract Parts Info" r:id="rId6" sheetId="10"/>
-    <sheet name="TC2-BU to Customer Contract" r:id="rId7" sheetId="9"/>
-    <sheet name="TC3-BU Contract Route" r:id="rId8" sheetId="11"/>
-    <sheet name="TC3.2-Supplier ShippingRoute" r:id="rId9" sheetId="7"/>
-    <sheet name="TC3.2-ETAnWeek" r:id="rId10" sheetId="8"/>
-    <sheet name="TC4-Supp to BU Contract" r:id="rId11" sheetId="12"/>
-    <sheet name="TC4-Contract Parts Info" r:id="rId12" sheetId="13"/>
-    <sheet name="TC5-BU Contract Route" r:id="rId13" sheetId="14"/>
-    <sheet name="TC6-Supplier Contract Route" r:id="rId14" sheetId="15"/>
-    <sheet name="TC9-BU Contract Route" r:id="rId15" sheetId="16"/>
-    <sheet name="TC20-Customer Request" r:id="rId16" sheetId="17"/>
-    <sheet name="TC21-BU Received Request" r:id="rId17" sheetId="18"/>
-    <sheet name="TC21-BU to Customer Contract" r:id="rId18" sheetId="22"/>
-    <sheet name="TC23-Sup Received Request (NEW)" r:id="rId19" sheetId="24"/>
-    <sheet name="TC23-Supplier to BU Contract" r:id="rId20" sheetId="21"/>
-    <sheet name="TC36-BU Receive Req Resub (NEW)" r:id="rId21" sheetId="46"/>
-    <sheet name="TC36-BU to Customer Contract" r:id="rId22" sheetId="28"/>
-    <sheet name="TC38-SUP Receive Req" r:id="rId23" sheetId="29"/>
-    <sheet name="TC38-SUP to BU Contract" r:id="rId24" sheetId="30"/>
-    <sheet name="TC41-CUS Reg Order (Firm)" r:id="rId25" sheetId="31"/>
-    <sheet name="TC41-CUS Reg Order (Date)" r:id="rId26" sheetId="32"/>
-    <sheet name="TC42-CUS Download CO" r:id="rId27" sheetId="33"/>
-    <sheet name="TC44-Autogen BU Sales Order" r:id="rId28" sheetId="34"/>
-    <sheet name="TC45-Autogen BU PO" r:id="rId29" sheetId="35"/>
-    <sheet name="TC46-Autogen SUP Sales Order" r:id="rId30" sheetId="36"/>
-    <sheet name="TC46-BU SO Delivery Plan" r:id="rId31" sheetId="37"/>
-    <sheet name="TC46-BU SO Delivery Plan (Date)" r:id="rId32" sheetId="38"/>
-    <sheet name="TC46-BU SO Price" r:id="rId33" sheetId="39"/>
-    <sheet name="TC47-SUP Upload Outbound Result" r:id="rId34" sheetId="40"/>
-    <sheet name="TC47-OutboundNo" r:id="rId35" sheetId="51"/>
-    <sheet name="TC52-CUS Check Cargo Tracking" r:id="rId36" sheetId="62"/>
-    <sheet name="TC52-Forecast Container" r:id="rId37" sheetId="68"/>
-    <sheet name="TC53-BU Check Cargo Tracking" r:id="rId38" sheetId="63"/>
-    <sheet name="TC54-Sup Check Cargo Tracking" r:id="rId39" sheetId="64"/>
-    <sheet name="TC59-Supplier Order Change" r:id="rId40" sheetId="41"/>
-    <sheet name="TC59-Supplier Order Change Date" r:id="rId41" sheetId="42"/>
-    <sheet name="TC60-SUP Order Change Request" r:id="rId42" sheetId="43"/>
-    <sheet name="TC62-Customer Approve Change" r:id="rId43" sheetId="65"/>
-    <sheet name="TC63-BU Check Change" r:id="rId44" sheetId="66"/>
-    <sheet name="TC64-Sup Check Change" r:id="rId45" sheetId="67"/>
-    <sheet name="TC69-Supplier Outbound" r:id="rId46" sheetId="48"/>
-    <sheet name="TC69-OutboundNo" r:id="rId47" sheetId="49"/>
-    <sheet name="TC70-Supplier Check SO" r:id="rId48" sheetId="50"/>
-    <sheet name="TC74-Supplier Seller GI Invoice" r:id="rId49" sheetId="44"/>
-    <sheet name="TC77-BU Seller GI Invoice" r:id="rId50" sheetId="45"/>
-    <sheet name="TC78-OutboundNo List" r:id="rId51" sheetId="52"/>
-    <sheet name="TC78-DC Inbound Details" r:id="rId52" sheetId="53"/>
-    <sheet name="TC79-Supplier Check SO" r:id="rId53" sheetId="54"/>
-    <sheet name="TC83-Inventory By Parts" r:id="rId54" sheetId="60"/>
-    <sheet name="TC84-Inventory By Package" r:id="rId55" sheetId="69"/>
-    <sheet name="TC85-DC Outbound" r:id="rId56" sheetId="56"/>
-    <sheet name="TC85-OutboundNo" r:id="rId57" sheetId="55"/>
-    <sheet name="TC86-BU Seller GI Invoice" r:id="rId58" sheetId="57"/>
-    <sheet name="TC91-Customer Inbound Details" r:id="rId59" sheetId="58"/>
-    <sheet name="TC91-OutboundNo" r:id="rId60" sheetId="59"/>
-    <sheet name="AutoIncrement" r:id="rId61" sheetId="2"/>
+    <sheet name="TC1-Request Add New" sheetId="1" r:id="rId1"/>
+    <sheet name="TC1" sheetId="3" r:id="rId2"/>
+    <sheet name="TC1.1&amp;3.1-Payment Terms" sheetId="4" r:id="rId3"/>
+    <sheet name="TC1.2-BU ShippingRoute" sheetId="5" r:id="rId4"/>
+    <sheet name="TC1.2-ETAnWeek" sheetId="6" r:id="rId5"/>
+    <sheet name="TC2-Contract Parts Info" sheetId="10" r:id="rId6"/>
+    <sheet name="TC2-BU to Customer Contract" sheetId="9" r:id="rId7"/>
+    <sheet name="TC3-BU Contract Route" sheetId="11" r:id="rId8"/>
+    <sheet name="TC3.2-Supplier ShippingRoute" sheetId="7" r:id="rId9"/>
+    <sheet name="TC3.2-ETAnWeek" sheetId="8" r:id="rId10"/>
+    <sheet name="TC4-Supp to BU Contract" sheetId="12" r:id="rId11"/>
+    <sheet name="TC4-Contract Parts Info" sheetId="13" r:id="rId12"/>
+    <sheet name="TC5-BU Contract Route" sheetId="14" r:id="rId13"/>
+    <sheet name="TC6-Supplier Contract Route" sheetId="15" r:id="rId14"/>
+    <sheet name="TC9-BU Contract Route" sheetId="16" r:id="rId15"/>
+    <sheet name="TC20-Customer Request" sheetId="17" r:id="rId16"/>
+    <sheet name="TC21-BU Received Request" sheetId="18" r:id="rId17"/>
+    <sheet name="TC21-BU to Customer Contract" sheetId="22" r:id="rId18"/>
+    <sheet name="TC23-Sup Received Request (NEW)" sheetId="24" r:id="rId19"/>
+    <sheet name="TC23-Supplier to BU Contract" sheetId="21" r:id="rId20"/>
+    <sheet name="TC36-BU Receive Req Resub (NEW)" sheetId="46" r:id="rId21"/>
+    <sheet name="TC36-BU to Customer Contract" sheetId="28" r:id="rId22"/>
+    <sheet name="TC38-SUP Receive Req" sheetId="29" r:id="rId23"/>
+    <sheet name="TC38-SUP to BU Contract" sheetId="30" r:id="rId24"/>
+    <sheet name="TC41-CUS Reg Order (Firm)" sheetId="31" r:id="rId25"/>
+    <sheet name="TC41-CUS Reg Order (Date)" sheetId="32" r:id="rId26"/>
+    <sheet name="TC42-CUS Download CO" sheetId="33" r:id="rId27"/>
+    <sheet name="TC44-Autogen BU Sales Order" sheetId="34" r:id="rId28"/>
+    <sheet name="TC45-Autogen BU PO" sheetId="35" r:id="rId29"/>
+    <sheet name="TC46-Autogen SUP Sales Order" sheetId="36" r:id="rId30"/>
+    <sheet name="TC46-BU SO Delivery Plan" sheetId="37" r:id="rId31"/>
+    <sheet name="TC46-BU SO Delivery Plan (Date)" sheetId="38" r:id="rId32"/>
+    <sheet name="TC46-BU SO Price" sheetId="39" r:id="rId33"/>
+    <sheet name="TC47-SUP Upload Outbound Result" sheetId="40" r:id="rId34"/>
+    <sheet name="TC47-OutboundNo" sheetId="51" r:id="rId35"/>
+    <sheet name="TC52-CUS Check Cargo Tracking" sheetId="62" r:id="rId36"/>
+    <sheet name="TC52-Forecast Container" sheetId="68" r:id="rId37"/>
+    <sheet name="TC53-BU Check Cargo Tracking" sheetId="63" r:id="rId38"/>
+    <sheet name="TC54-Sup Check Cargo Tracking" sheetId="64" r:id="rId39"/>
+    <sheet name="TC59-Supplier Order Change" sheetId="41" r:id="rId40"/>
+    <sheet name="TC59-Supplier Order Change Date" sheetId="42" r:id="rId41"/>
+    <sheet name="TC60-SUP Order Change Request" sheetId="43" r:id="rId42"/>
+    <sheet name="TC62-Customer Approve Change" sheetId="65" r:id="rId43"/>
+    <sheet name="TC63-BU Check Change" sheetId="66" r:id="rId44"/>
+    <sheet name="TC64-Sup Check Change" sheetId="67" r:id="rId45"/>
+    <sheet name="TC69-Supplier Outbound" sheetId="48" r:id="rId46"/>
+    <sheet name="TC69-OutboundNo" sheetId="49" r:id="rId47"/>
+    <sheet name="TC70-Supplier Check SO" sheetId="50" r:id="rId48"/>
+    <sheet name="TC74-Supplier Seller GI Invoice" sheetId="44" r:id="rId49"/>
+    <sheet name="TC77-BU Seller GI Invoice" sheetId="45" r:id="rId50"/>
+    <sheet name="TC78-OutboundNo List" sheetId="52" r:id="rId51"/>
+    <sheet name="TC78-DC Inbound Details" sheetId="53" r:id="rId52"/>
+    <sheet name="TC79-Supplier Check SO" sheetId="54" r:id="rId53"/>
+    <sheet name="TC83-Inventory By Parts" sheetId="60" r:id="rId54"/>
+    <sheet name="TC84-Inventory By Package" sheetId="69" r:id="rId55"/>
+    <sheet name="TC85-DC Outbound" sheetId="56" r:id="rId56"/>
+    <sheet name="TC85-OutboundNo" sheetId="55" r:id="rId57"/>
+    <sheet name="TC86-BU Seller GI Invoice" sheetId="57" r:id="rId58"/>
+    <sheet name="TC91-Customer Inbound Details" sheetId="58" r:id="rId59"/>
+    <sheet name="TC91-OutboundNo" sheetId="59" r:id="rId60"/>
+    <sheet name="AutoIncrement" sheetId="2" r:id="rId61"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId62"/>
@@ -82,38 +82,38 @@
     <externalReference r:id="rId65"/>
   </externalReferences>
   <definedNames>
-    <definedName hidden="1" localSheetId="40" name="_xlnm._FilterDatabase">'TC59-Supplier Order Change Date'!$B$1:$F$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="40" hidden="1">'TC59-Supplier Order Change Date'!$B$1:$F$4</definedName>
     <definedName name="activeFlagListArr">[1]activeFlagListArr!$A$1:$A$2</definedName>
     <definedName name="activeFlagStrArr">[2]activeFlagStrArr!$A$1:$A$2</definedName>
-    <definedName localSheetId="35" name="CURRENCY_CODE">[3]CURRENCY_CODE!$A$1:$A$13</definedName>
-    <definedName localSheetId="37" name="CURRENCY_CODE">[3]CURRENCY_CODE!$A$1:$A$13</definedName>
-    <definedName localSheetId="38" name="CURRENCY_CODE">[3]CURRENCY_CODE!$A$1:$A$13</definedName>
+    <definedName name="CURRENCY_CODE" localSheetId="35">[3]CURRENCY_CODE!$A$1:$A$13</definedName>
+    <definedName name="CURRENCY_CODE" localSheetId="37">[3]CURRENCY_CODE!$A$1:$A$13</definedName>
+    <definedName name="CURRENCY_CODE" localSheetId="38">[3]CURRENCY_CODE!$A$1:$A$13</definedName>
     <definedName name="CURRENCY_CODE">[4]CURRENCY_CODE!$A$1:$A$13</definedName>
     <definedName name="findAllUomArr">[1]findAllUomArr!$A$1:$A$29</definedName>
-    <definedName localSheetId="35" name="PAIRED_FLAG">#REF!</definedName>
-    <definedName localSheetId="37" name="PAIRED_FLAG">#REF!</definedName>
-    <definedName localSheetId="38" name="PAIRED_FLAG">#REF!</definedName>
+    <definedName name="PAIRED_FLAG" localSheetId="35">#REF!</definedName>
+    <definedName name="PAIRED_FLAG" localSheetId="37">#REF!</definedName>
+    <definedName name="PAIRED_FLAG" localSheetId="38">#REF!</definedName>
     <definedName name="PAIRED_FLAG">#REF!</definedName>
-    <definedName localSheetId="35" name="PAIRED_ORDER_FLAG">#REF!</definedName>
-    <definedName localSheetId="37" name="PAIRED_ORDER_FLAG">#REF!</definedName>
-    <definedName localSheetId="38" name="PAIRED_ORDER_FLAG">#REF!</definedName>
+    <definedName name="PAIRED_ORDER_FLAG" localSheetId="35">#REF!</definedName>
+    <definedName name="PAIRED_ORDER_FLAG" localSheetId="37">#REF!</definedName>
+    <definedName name="PAIRED_ORDER_FLAG" localSheetId="38">#REF!</definedName>
     <definedName name="PAIRED_ORDER_FLAG">#REF!</definedName>
     <definedName name="pairedPartsFlagStrArr">[2]pairedPartsFlagStrArr!$A$1:$A$2</definedName>
     <definedName name="partsTypeArr">[1]partsTypeArr!$A$1:$A$4</definedName>
-    <definedName localSheetId="35" name="REPACKING_TYPE">#REF!</definedName>
-    <definedName localSheetId="37" name="REPACKING_TYPE">#REF!</definedName>
-    <definedName localSheetId="38" name="REPACKING_TYPE">#REF!</definedName>
+    <definedName name="REPACKING_TYPE" localSheetId="35">#REF!</definedName>
+    <definedName name="REPACKING_TYPE" localSheetId="37">#REF!</definedName>
+    <definedName name="REPACKING_TYPE" localSheetId="38">#REF!</definedName>
     <definedName name="REPACKING_TYPE">[4]REPACKING_TYPE!$A$1:$A$3</definedName>
     <definedName name="rolledPartsFlagArr">[1]rolledPartsFlagArr!$A$1:$A$2</definedName>
     <definedName name="rolledPartsUomArr">[1]rolledPartsUomArr!$A$1:$A$29</definedName>
-    <definedName localSheetId="35" name="UOM_CODE">#REF!</definedName>
-    <definedName localSheetId="37" name="UOM_CODE">#REF!</definedName>
-    <definedName localSheetId="38" name="UOM_CODE">#REF!</definedName>
+    <definedName name="UOM_CODE" localSheetId="35">#REF!</definedName>
+    <definedName name="UOM_CODE" localSheetId="37">#REF!</definedName>
+    <definedName name="UOM_CODE" localSheetId="38">#REF!</definedName>
     <definedName name="UOM_CODE">#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="391">
   <si>
     <t>ShortCode1</t>
   </si>
@@ -956,9 +956,6 @@
     <t>PK-SUP-scenario9-003</t>
   </si>
   <si>
-    <t>Nov 14, 2023</t>
-  </si>
-  <si>
     <t>Nov 16, 2023</t>
   </si>
   <si>
@@ -1295,12 +1292,6 @@
     <t>o-PK-SUP-POC-231012002</t>
   </si>
   <si>
-    <t>PKS2310025</t>
-  </si>
-  <si>
-    <t>PKS2310026</t>
-  </si>
-  <si>
     <t>Package No</t>
   </si>
   <si>
@@ -1311,6 +1302,9 @@
   </si>
   <si>
     <t>PNA2310005</t>
+  </si>
+  <si>
+    <t>Nov 22, 2023</t>
   </si>
 </sst>
 </file>
@@ -1431,101 +1425,101 @@
     </border>
   </borders>
   <cellStyleXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="43"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="36">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="3" xfId="0">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="9" xfId="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="6" numFmtId="3" xfId="0">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="9" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="3" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="167" xfId="2">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="6" numFmtId="168" xfId="2">
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="170" xfId="4"/>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="169" xfId="0">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="171" xfId="0"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle builtinId="3" name="Comma" xfId="4"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Comma" xfId="4" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 2" xfId="2" xr:uid="{9620B1EC-23CB-476C-A2A7-7D32C42EBD30}"/>
     <cellStyle name="Normal 6 2" xfId="3" xr:uid="{7F18E85A-5FD7-4515-B1EA-2F2A6E17A45E}"/>
     <cellStyle name="常规 2" xfId="1" xr:uid="{11C250DD-8E17-4907-B350-1E8C975650C5}"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2141,10 +2135,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -2179,7 +2173,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2214,7 +2208,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2308,21 +2302,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2339,7 +2333,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -2391,29 +2385,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="6" width="20.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="6" width="15.77734375" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" style="6" width="20.77734375" collapsed="true"/>
-    <col min="5" max="8" customWidth="true" style="6" width="15.77734375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="6" width="20.77734375" collapsed="true"/>
-    <col min="10" max="16" customWidth="true" style="6" width="15.77734375" collapsed="true"/>
-    <col min="17" max="16384" style="6" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="20.77734375" style="6" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.77734375" style="6" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="20.77734375" style="6" customWidth="1" collapsed="1"/>
+    <col min="5" max="8" width="15.77734375" style="6" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.77734375" style="6" customWidth="1" collapsed="1"/>
+    <col min="10" max="16" width="15.77734375" style="6" customWidth="1" collapsed="1"/>
+    <col min="17" max="16384" width="8.88671875" style="6" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -2601,14 +2595,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C21FEEA-1F2D-49E6-8055-702BD3BCDFE2}">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C21FEEA-1F2D-49E6-8055-702BD3BCDFE2}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
@@ -2616,8 +2610,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.77734375" collapsed="true"/>
-    <col min="2" max="15" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="1" max="1" width="25.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="15" width="15.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -2716,23 +2710,23 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4BE1A7-9914-4D3E-B6DE-DFFF17DDF6D0}">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4BE1A7-9914-4D3E-B6DE-DFFF17DDF6D0}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="4.77734375" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="25.77734375" collapsed="true"/>
-    <col min="4" max="14" customWidth="true" width="18.77734375" collapsed="true"/>
+    <col min="1" max="1" width="4.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="25.77734375" customWidth="1" collapsed="1"/>
+    <col min="4" max="14" width="18.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -2784,7 +2778,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C2" t="str">
         <f>"PKSUP-PKTTAP-"&amp;AutoIncrement!C2&amp;"-0"&amp;AutoIncrement!A2</f>
@@ -2827,13 +2821,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A00FF8C-9113-4ADC-B8A3-868C085422B7}">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A00FF8C-9113-4ADC-B8A3-868C085422B7}">
+  <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
@@ -2841,15 +2835,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="4.77734375" collapsed="true"/>
-    <col min="2" max="4" customWidth="true" width="20.77734375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="25.77734375" collapsed="true"/>
-    <col min="6" max="10" customWidth="true" width="15.77734375" collapsed="true"/>
-    <col min="12" max="12" width="8.88671875" collapsed="true"/>
-    <col min="31" max="16384" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="4.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="20.77734375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="25.77734375" customWidth="1" collapsed="1"/>
+    <col min="6" max="10" width="15.77734375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="8.88671875" collapsed="1"/>
+    <col min="31" max="16384" width="8.88671875" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>27</v>
       </c>
@@ -2975,14 +2969,14 @@
       <c r="J4" s="16"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A635215-D865-4792-901A-69EC3D54CB7A}">
-  <dimension ref="A1:M4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A635215-D865-4792-901A-69EC3D54CB7A}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
@@ -2990,13 +2984,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="20.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.77734375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.77734375" collapsed="true"/>
-    <col min="5" max="8" customWidth="true" width="15.77734375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="20.77734375" collapsed="true"/>
-    <col min="10" max="12" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="1" max="1" width="15.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.77734375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.77734375" customWidth="1" collapsed="1"/>
+    <col min="5" max="8" width="15.77734375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.77734375" customWidth="1" collapsed="1"/>
+    <col min="10" max="12" width="15.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -3158,13 +3152,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF55D3EB-FD6F-4467-A298-9C9BA6F25DBB}">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF55D3EB-FD6F-4467-A298-9C9BA6F25DBB}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
@@ -3172,11 +3166,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="20.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.77734375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.77734375" collapsed="true"/>
-    <col min="5" max="7" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="1" max="1" width="15.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.77734375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.77734375" customWidth="1" collapsed="1"/>
+    <col min="5" max="7" width="15.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -3275,13 +3269,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E403EE8-8C1F-4E1E-AA64-4A79D4DB0253}">
-  <dimension ref="A1:M4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E403EE8-8C1F-4E1E-AA64-4A79D4DB0253}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
@@ -3289,13 +3283,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="20.77734375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.77734375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.77734375" collapsed="true"/>
-    <col min="5" max="8" customWidth="true" width="15.77734375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="20.77734375" collapsed="true"/>
-    <col min="10" max="12" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="1" max="1" width="15.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.77734375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.77734375" customWidth="1" collapsed="1"/>
+    <col min="5" max="8" width="15.77734375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20.77734375" customWidth="1" collapsed="1"/>
+    <col min="10" max="12" width="15.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -3412,22 +3406,22 @@
       <c r="J4" s="7"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1543C1E1-9487-4769-918B-43BE22CAAF0B}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1543C1E1-9487-4769-918B-43BE22CAAF0B}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" customWidth="true" style="6" width="15.77734375" collapsed="true"/>
-    <col min="4" max="16384" style="6" width="8.88671875" collapsed="true"/>
+    <col min="1" max="3" width="15.77734375" style="6" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="8.88671875" style="6" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -3476,24 +3470,24 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CDBD6F2-35F7-4FDA-96CA-A9095045351C}">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CDBD6F2-35F7-4FDA-96CA-A9095045351C}">
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="80" zoomScaleNormal="80">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="2" max="9" customWidth="true" width="15.77734375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="22.6640625" collapsed="true"/>
+    <col min="1" max="1" width="23" customWidth="1" collapsed="1"/>
+    <col min="2" max="9" width="15.77734375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -3629,13 +3623,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA32C3B8-47A0-4792-B0C5-BB96E61C0725}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA32C3B8-47A0-4792-B0C5-BB96E61C0725}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -3643,9 +3637,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.77734375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.21875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.88671875" collapsed="true"/>
+    <col min="2" max="2" width="20.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -3667,24 +3661,24 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C2" t="str">
         <f>"RD-"&amp;AutoIncrement!B2&amp;"-"&amp;AutoIncrement!A2</f>
         <v>RD-E-02</v>
       </c>
       <c r="D2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4720C32-AF2E-4F8E-89E7-198E2A9CBB44}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4720C32-AF2E-4F8E-89E7-198E2A9CBB44}">
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
@@ -3692,7 +3686,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="28.109375" collapsed="true"/>
+    <col min="1" max="1" width="28.109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -3719,13 +3713,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C965315-2958-4E59-B934-7C2E7EC38B33}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C965315-2958-4E59-B934-7C2E7EC38B33}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -3733,7 +3727,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="22.77734375" collapsed="true"/>
+    <col min="2" max="2" width="22.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -3744,7 +3738,7 @@
         <v>28</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -3754,13 +3748,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B4532A-6C80-4B65-856D-22F77F1A27B1}">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B4532A-6C80-4B65-856D-22F77F1A27B1}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -3768,12 +3762,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
-    <col min="4" max="12" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="28.77734375" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="27.6640625" collapsed="true"/>
+    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="12" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="28.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="27.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -3828,7 +3822,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C2" t="str">
         <f>"PKSUP-PKTTAP-"&amp;AutoIncrement!D2&amp;"-0"&amp;AutoIncrement!A2&amp;"-NEW"</f>
@@ -3870,17 +3864,17 @@
         <v>106</v>
       </c>
       <c r="O2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2D9605-759A-40B5-8A1E-B3F890190A83}">
-  <dimension ref="A1:S4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2D9605-759A-40B5-8A1E-B3F890190A83}">
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="Q17" sqref="Q17"/>
@@ -3888,12 +3882,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.77734375" collapsed="true"/>
-    <col min="2" max="17" customWidth="true" width="15.77734375" collapsed="true"/>
-    <col min="18" max="16384" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="25.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="17" width="15.77734375" customWidth="1" collapsed="1"/>
+    <col min="18" max="16384" width="8.88671875" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>91</v>
       </c>
@@ -4093,14 +4087,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7197938-4732-4F77-A314-C8FDF3D7382E}">
-  <dimension ref="A1:R2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7197938-4732-4F77-A314-C8FDF3D7382E}">
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
@@ -4108,13 +4102,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
-    <col min="4" max="13" customWidth="true" width="15.77734375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="15" max="16" customWidth="true" width="15.77734375" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="33.33203125" collapsed="true"/>
+    <col min="1" max="1" width="10.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="13" width="15.77734375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="15.77734375" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="33.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -4175,7 +4169,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C2" t="str">
         <f>"PKTTAP-PKCUS-"&amp;AutoIncrement!E2&amp;"-0"&amp;AutoIncrement!A2</f>
@@ -4224,17 +4218,17 @@
         <v>106</v>
       </c>
       <c r="Q2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A78B61-8D30-4279-BF5F-C888C349BF31}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A78B61-8D30-4279-BF5F-C888C349BF31}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -4242,8 +4236,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="28.109375" collapsed="true"/>
-    <col min="2" max="5" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="1" max="1" width="28.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="5" width="15.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -4318,13 +4312,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FA47E05-B85D-4AE2-87E4-941E5A55E58A}">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FA47E05-B85D-4AE2-87E4-941E5A55E58A}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M14" sqref="M14"/>
@@ -4332,12 +4326,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
-    <col min="4" max="12" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="28.77734375" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="24.88671875" collapsed="true"/>
+    <col min="2" max="2" width="21.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="12" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="28.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.77734375" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="24.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -4392,7 +4386,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C2" t="str">
         <f>'TC23-Supplier to BU Contract'!C2</f>
@@ -4434,17 +4428,17 @@
         <v>106</v>
       </c>
       <c r="O2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5638E0D3-4FBE-457D-8595-037419E8E6CB}">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5638E0D3-4FBE-457D-8595-037419E8E6CB}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
@@ -4452,7 +4446,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="1" max="4" width="15.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -4512,49 +4506,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71D6F661-EB37-4576-9A5B-734075C2BA0D}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.5546875" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="str">
-        <f ca="1">TEXT(EOMONTH(TODAY(),1),"dd MMM yyyy")</f>
-        <v>30 Nov 2023</v>
-      </c>
-      <c r="B2" t="str">
-        <f ca="1">TEXT(EOMONTH(TODAY(),2),"dd MMM yyyy")</f>
-        <v>31 Dec 2023</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F481100E-C4A6-4B18-8C5B-E65FDA7323E3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71D6F661-EB37-4576-9A5B-734075C2BA0D}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4563,7 +4520,44 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="str">
+        <f ca="1">TEXT(EOMONTH(TODAY(),1),"dd MMM yyyy")</f>
+        <v>31 Dec 2023</v>
+      </c>
+      <c r="B2" t="str">
+        <f ca="1">TEXT(EOMONTH(TODAY(),2),"dd MMM yyyy")</f>
+        <v>31 Jan 2024</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F481100E-C4A6-4B18-8C5B-E65FDA7323E3}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -4573,17 +4567,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CCB6063-2CFD-4337-A08A-CB19FD0F33E3}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CCB6063-2CFD-4337-A08A-CB19FD0F33E3}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
@@ -4591,7 +4585,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -4601,17 +4595,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC31B8AD-898A-401A-8D76-A16ABAB2BE94}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC31B8AD-898A-401A-8D76-A16ABAB2BE94}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -4619,7 +4613,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.109375" collapsed="true"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -4629,17 +4623,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC2FF1C-7C07-4C59-9D46-A8B22CD038DD}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC2FF1C-7C07-4C59-9D46-A8B22CD038DD}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
@@ -4647,7 +4641,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="1" max="7" width="15.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -4697,13 +4691,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD524ABC-71B5-4CAC-BBAD-A8CFB20FB54D}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD524ABC-71B5-4CAC-BBAD-A8CFB20FB54D}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -4718,17 +4712,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303D3629-A54E-41F9-9DFA-F433B1BE8C74}">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303D3629-A54E-41F9-9DFA-F433B1BE8C74}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
@@ -4736,9 +4730,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" bestFit="true" customWidth="true" width="15.109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="36.33203125" collapsed="true"/>
+    <col min="1" max="5" width="15.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -4764,7 +4758,7 @@
         <v>238</v>
       </c>
     </row>
-    <row ht="57.6" r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>500</v>
       </c>
@@ -4787,7 +4781,7 @@
         <v>239</v>
       </c>
     </row>
-    <row ht="57.6" r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -4804,7 +4798,7 @@
         <v>800</v>
       </c>
       <c r="F3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>246</v>
@@ -4832,24 +4826,24 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DF16506-5648-469A-9B60-042110BEB0F4}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DF16506-5648-469A-9B60-042110BEB0F4}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="25.6640625" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" width="25.77734375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="25.21875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="26.77734375" collapsed="true"/>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="25.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -4877,7 +4871,7 @@
         <v>274</v>
       </c>
       <c r="B2" t="s">
-        <v>275</v>
+        <v>390</v>
       </c>
       <c r="C2" t="s">
         <v>186</v>
@@ -4894,10 +4888,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>274</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>390</v>
       </c>
       <c r="C3" t="s">
         <v>186</v>
@@ -4906,7 +4900,7 @@
         <v>186</v>
       </c>
       <c r="E3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F3" t="s">
         <v>241</v>
@@ -4914,16 +4908,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>186</v>
+        <v>274</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>390</v>
       </c>
       <c r="C4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D4" t="s">
         <v>276</v>
-      </c>
-      <c r="D4" t="s">
-        <v>277</v>
       </c>
       <c r="E4" t="s">
         <v>186</v>
@@ -4931,13 +4925,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D255DFB-2F74-4695-A9BE-4F3A79219025}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D255DFB-2F74-4695-A9BE-4F3A79219025}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -4978,13 +4972,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9BF608A-498D-4638-9EB0-6E6796BB101C}">
-  <dimension ref="A1:AA4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9BF608A-498D-4638-9EB0-6E6796BB101C}">
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3:F3"/>
@@ -4992,31 +4986,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="24.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.88671875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.88671875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.5546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
-    <col min="7" max="8" bestFit="true" customWidth="true" width="10.77734375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.88671875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="15.21875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.6640625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="20.77734375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="17.88671875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="14.5546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="16.77734375" collapsed="true"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="19.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="17" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="12.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
@@ -5122,11 +5116,11 @@
       </c>
       <c r="G2" t="str">
         <f ca="1">TEXT(TODAY(),"dd MMM yyyy")</f>
-        <v>19 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
       <c r="H2" t="str">
         <f ca="1">TEXT(TODAY()+1,"dd MMM yyyy")</f>
-        <v>20 Oct 2023</v>
+        <v>02 Nov 2023</v>
       </c>
       <c r="I2" t="s">
         <v>197</v>
@@ -5179,9 +5173,9 @@
       <c r="Y2">
         <v>20</v>
       </c>
-      <c r="Z2" t="e">
+      <c r="Z2" t="str">
         <f ca="1">TEXT(H2, "mmm dd, yyyyy")</f>
-        <v>#VALUE!</v>
+        <v>Nov 02, 2023</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
@@ -5206,12 +5200,12 @@
         <v>88</v>
       </c>
       <c r="G3" t="str">
-        <f ca="1" ref="G3:G4" si="0" t="shared">TEXT(TODAY(),"dd MMM yyyy")</f>
-        <v>19 Oct 2023</v>
+        <f t="shared" ref="G3:G4" ca="1" si="0">TEXT(TODAY(),"dd MMM yyyy")</f>
+        <v>01 Nov 2023</v>
       </c>
       <c r="H3" t="str">
-        <f ca="1" ref="H3:H4" si="1" t="shared">TEXT(TODAY()+1,"dd MMM yyyy")</f>
-        <v>20 Oct 2023</v>
+        <f t="shared" ref="H3:H4" ca="1" si="1">TEXT(TODAY()+1,"dd MMM yyyy")</f>
+        <v>02 Nov 2023</v>
       </c>
       <c r="I3" t="s">
         <v>198</v>
@@ -5231,9 +5225,9 @@
       <c r="T3">
         <v>100</v>
       </c>
-      <c r="Z3" t="e">
-        <f ca="1" ref="Z3:Z4" si="2" t="shared">TEXT(H3, "mmm dd, yyyyy")</f>
-        <v>#VALUE!</v>
+      <c r="Z3" t="str">
+        <f t="shared" ref="Z3:Z4" ca="1" si="2">TEXT(H3, "mmm dd, yyyyy")</f>
+        <v>Nov 02, 2023</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
@@ -5258,12 +5252,12 @@
         <v>82</v>
       </c>
       <c r="G4" t="str">
-        <f ca="1" si="0" t="shared"/>
-        <v>19 Oct 2023</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>01 Nov 2023</v>
       </c>
       <c r="H4" t="str">
-        <f ca="1" si="1" t="shared"/>
-        <v>20 Oct 2023</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>02 Nov 2023</v>
       </c>
       <c r="I4" t="s">
         <v>199</v>
@@ -5287,7 +5281,7 @@
         <v>1000</v>
       </c>
       <c r="P4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="Q4" t="s">
         <v>219</v>
@@ -5301,19 +5295,19 @@
       <c r="T4">
         <v>100</v>
       </c>
-      <c r="Z4" t="e">
-        <f ca="1" si="2" t="shared"/>
-        <v>#VALUE!</v>
+      <c r="Z4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Nov 02, 2023</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4628A4-4D14-4796-80AA-C6878E4D497C}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4628A4-4D14-4796-80AA-C6878E4D497C}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
@@ -5321,8 +5315,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.44140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="27.77734375" collapsed="true"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -5339,7 +5333,7 @@
         <v>o-PK-SUP-POC-E-02-001</v>
       </c>
       <c r="B2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -5348,17 +5342,17 @@
         <v>o-PK-SUP-POC-E-02-002</v>
       </c>
       <c r="B3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2367BF5F-F59C-4A60-813D-215BE940932D}">
-  <dimension ref="A1:AA4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2367BF5F-F59C-4A60-813D-215BE940932D}">
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -5366,9 +5360,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" customWidth="true" style="6" width="25.6640625" collapsed="true"/>
-    <col min="3" max="26" customWidth="true" style="6" width="20.6640625" collapsed="true"/>
-    <col min="27" max="16384" style="6" width="8.88671875" collapsed="true"/>
+    <col min="1" max="2" width="25.6640625" style="6" customWidth="1" collapsed="1"/>
+    <col min="3" max="26" width="20.6640625" style="6" customWidth="1" collapsed="1"/>
+    <col min="27" max="16384" width="8.88671875" style="6" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
@@ -5379,76 +5373,76 @@
         <v>196</v>
       </c>
       <c r="C1" s="33" t="s">
+        <v>287</v>
+      </c>
+      <c r="D1" s="33" t="s">
         <v>288</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="E1" s="33" t="s">
         <v>289</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="F1" s="33" t="s">
         <v>290</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="G1" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="H1" s="33" t="s">
         <v>292</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="I1" s="33" t="s">
         <v>293</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="J1" s="33" t="s">
         <v>294</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="K1" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="L1" s="33" t="s">
         <v>296</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="M1" s="33" t="s">
         <v>297</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="N1" s="33" t="s">
         <v>298</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="O1" s="33" t="s">
         <v>299</v>
       </c>
-      <c r="O1" s="33" t="s">
+      <c r="P1" s="33" t="s">
         <v>300</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="Q1" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="R1" s="33" t="s">
+        <v>300</v>
+      </c>
+      <c r="S1" s="33" t="s">
         <v>301</v>
       </c>
-      <c r="Q1" s="33" t="s">
-        <v>300</v>
-      </c>
-      <c r="R1" s="33" t="s">
+      <c r="T1" s="33" t="s">
+        <v>302</v>
+      </c>
+      <c r="U1" s="33" t="s">
         <v>301</v>
       </c>
-      <c r="S1" s="33" t="s">
+      <c r="V1" s="33" t="s">
         <v>302</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="W1" s="33" t="s">
         <v>303</v>
       </c>
-      <c r="U1" s="33" t="s">
-        <v>302</v>
-      </c>
-      <c r="V1" s="33" t="s">
-        <v>303</v>
-      </c>
-      <c r="W1" s="33" t="s">
+      <c r="X1" s="33" t="s">
         <v>304</v>
       </c>
-      <c r="X1" s="33" t="s">
+      <c r="Y1" s="33" t="s">
         <v>305</v>
       </c>
-      <c r="Y1" s="33" t="s">
+      <c r="Z1" s="33" t="s">
         <v>306</v>
-      </c>
-      <c r="Z1" s="33" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
@@ -5461,76 +5455,76 @@
         <v>C-20230628001</v>
       </c>
       <c r="C2" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="D2" s="33" t="s">
         <v>308</v>
       </c>
-      <c r="D2" s="33" t="s">
-        <v>309</v>
-      </c>
       <c r="E2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="O2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="S2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="T2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="U2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="V2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="W2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="X2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Y2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Z2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
@@ -5543,76 +5537,76 @@
         <v>SEGU5069987</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="O3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="S3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="T3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="U3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="V3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="W3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="X3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Y3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Z3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
@@ -5625,86 +5619,86 @@
         <v>C-20230628002</v>
       </c>
       <c r="C4" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="D4" s="33" t="s">
         <v>308</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>309</v>
-      </c>
       <c r="E4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="O4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="S4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="T4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="U4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="V4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="W4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="X4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Y4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Z4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF562A4D-D205-46B2-8728-400E42E0BFBC}">
-  <dimension ref="A1:R2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF562A4D-D205-46B2-8728-400E42E0BFBC}">
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
@@ -5712,10 +5706,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="20" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="1" max="20" width="15.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" ht="86.4" r="1" s="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="7" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>190</v>
       </c>
@@ -5723,49 +5717,49 @@
         <v>196</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>347</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>348</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>349</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>350</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>351</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>353</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>356</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>357</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>359</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -5778,59 +5772,59 @@
         <v>SEGU5069987</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="K2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="M2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="N2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="O2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="P2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="Q2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B99E25-E666-4F60-8638-591CD3B35C4F}">
-  <dimension ref="A1:AA4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B99E25-E666-4F60-8638-591CD3B35C4F}">
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
@@ -5838,9 +5832,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" customWidth="true" style="6" width="25.6640625" collapsed="true"/>
-    <col min="3" max="26" customWidth="true" style="6" width="20.6640625" collapsed="true"/>
-    <col min="27" max="16384" style="6" width="8.88671875" collapsed="true"/>
+    <col min="1" max="2" width="25.6640625" style="6" customWidth="1" collapsed="1"/>
+    <col min="3" max="26" width="20.6640625" style="6" customWidth="1" collapsed="1"/>
+    <col min="27" max="16384" width="8.88671875" style="6" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
@@ -5851,76 +5845,76 @@
         <v>196</v>
       </c>
       <c r="C1" s="33" t="s">
+        <v>287</v>
+      </c>
+      <c r="D1" s="33" t="s">
         <v>288</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="E1" s="33" t="s">
         <v>289</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="F1" s="33" t="s">
         <v>290</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="G1" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="H1" s="33" t="s">
         <v>292</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="I1" s="33" t="s">
         <v>293</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="J1" s="33" t="s">
         <v>294</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="K1" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="L1" s="33" t="s">
         <v>296</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="M1" s="33" t="s">
         <v>297</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="N1" s="33" t="s">
         <v>298</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="O1" s="33" t="s">
         <v>299</v>
       </c>
-      <c r="O1" s="33" t="s">
+      <c r="P1" s="33" t="s">
         <v>300</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="Q1" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="R1" s="33" t="s">
+        <v>300</v>
+      </c>
+      <c r="S1" s="33" t="s">
         <v>301</v>
       </c>
-      <c r="Q1" s="33" t="s">
-        <v>300</v>
-      </c>
-      <c r="R1" s="33" t="s">
+      <c r="T1" s="33" t="s">
+        <v>302</v>
+      </c>
+      <c r="U1" s="33" t="s">
         <v>301</v>
       </c>
-      <c r="S1" s="33" t="s">
+      <c r="V1" s="33" t="s">
         <v>302</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="W1" s="33" t="s">
         <v>303</v>
       </c>
-      <c r="U1" s="33" t="s">
-        <v>302</v>
-      </c>
-      <c r="V1" s="33" t="s">
-        <v>303</v>
-      </c>
-      <c r="W1" s="33" t="s">
+      <c r="X1" s="33" t="s">
         <v>304</v>
       </c>
-      <c r="X1" s="33" t="s">
+      <c r="Y1" s="33" t="s">
         <v>305</v>
       </c>
-      <c r="Y1" s="33" t="s">
+      <c r="Z1" s="33" t="s">
         <v>306</v>
-      </c>
-      <c r="Z1" s="33" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
@@ -5933,76 +5927,76 @@
         <v>C-20230628001</v>
       </c>
       <c r="C2" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="D2" s="33" t="s">
         <v>308</v>
       </c>
-      <c r="D2" s="33" t="s">
-        <v>309</v>
-      </c>
       <c r="E2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="O2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="S2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="T2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="U2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="V2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="W2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="X2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Y2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Z2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
@@ -6015,76 +6009,76 @@
         <v>SEGU5069987</v>
       </c>
       <c r="C3" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="D3" s="33" t="s">
         <v>308</v>
       </c>
-      <c r="D3" s="33" t="s">
-        <v>309</v>
-      </c>
       <c r="E3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="O3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="S3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="T3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="U3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="V3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="W3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="X3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Y3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Z3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
@@ -6097,86 +6091,86 @@
         <v>C-20230628002</v>
       </c>
       <c r="C4" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="D4" s="33" t="s">
         <v>308</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>309</v>
-      </c>
       <c r="E4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="O4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="S4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="T4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="U4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="V4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="W4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="X4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Y4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Z4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F59E7B6-CB99-45F2-915F-3BD483CEB83C}">
-  <dimension ref="A1:AA4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F59E7B6-CB99-45F2-915F-3BD483CEB83C}">
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
@@ -6184,9 +6178,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" customWidth="true" style="6" width="25.6640625" collapsed="true"/>
-    <col min="3" max="26" customWidth="true" style="6" width="20.6640625" collapsed="true"/>
-    <col min="27" max="16384" style="6" width="8.88671875" collapsed="true"/>
+    <col min="1" max="2" width="25.6640625" style="6" customWidth="1" collapsed="1"/>
+    <col min="3" max="26" width="20.6640625" style="6" customWidth="1" collapsed="1"/>
+    <col min="27" max="16384" width="8.88671875" style="6" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
@@ -6197,76 +6191,76 @@
         <v>196</v>
       </c>
       <c r="C1" s="33" t="s">
+        <v>287</v>
+      </c>
+      <c r="D1" s="33" t="s">
         <v>288</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="E1" s="33" t="s">
         <v>289</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="F1" s="33" t="s">
         <v>290</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="G1" s="33" t="s">
         <v>291</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="H1" s="33" t="s">
         <v>292</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="I1" s="33" t="s">
         <v>293</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="J1" s="33" t="s">
         <v>294</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="K1" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="L1" s="33" t="s">
         <v>296</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="M1" s="33" t="s">
         <v>297</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="N1" s="33" t="s">
         <v>298</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="O1" s="33" t="s">
         <v>299</v>
       </c>
-      <c r="O1" s="33" t="s">
+      <c r="P1" s="33" t="s">
         <v>300</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="Q1" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="R1" s="33" t="s">
+        <v>300</v>
+      </c>
+      <c r="S1" s="33" t="s">
         <v>301</v>
       </c>
-      <c r="Q1" s="33" t="s">
-        <v>300</v>
-      </c>
-      <c r="R1" s="33" t="s">
+      <c r="T1" s="33" t="s">
+        <v>302</v>
+      </c>
+      <c r="U1" s="33" t="s">
         <v>301</v>
       </c>
-      <c r="S1" s="33" t="s">
+      <c r="V1" s="33" t="s">
         <v>302</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="W1" s="33" t="s">
         <v>303</v>
       </c>
-      <c r="U1" s="33" t="s">
-        <v>302</v>
-      </c>
-      <c r="V1" s="33" t="s">
-        <v>303</v>
-      </c>
-      <c r="W1" s="33" t="s">
+      <c r="X1" s="33" t="s">
         <v>304</v>
       </c>
-      <c r="X1" s="33" t="s">
+      <c r="Y1" s="33" t="s">
         <v>305</v>
       </c>
-      <c r="Y1" s="33" t="s">
+      <c r="Z1" s="33" t="s">
         <v>306</v>
-      </c>
-      <c r="Z1" s="33" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
@@ -6279,76 +6273,76 @@
         <v>C-20230628001</v>
       </c>
       <c r="C2" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="D2" s="33" t="s">
         <v>308</v>
       </c>
-      <c r="D2" s="33" t="s">
-        <v>309</v>
-      </c>
       <c r="E2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="O2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="S2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="T2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="U2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="V2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="W2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="X2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Y2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Z2" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
@@ -6361,76 +6355,76 @@
         <v>SEGU5069987</v>
       </c>
       <c r="C3" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="D3" s="33" t="s">
         <v>308</v>
       </c>
-      <c r="D3" s="33" t="s">
-        <v>309</v>
-      </c>
       <c r="E3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="O3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="S3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="T3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="U3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="V3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="W3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="X3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Y3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Z3" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
@@ -6443,95 +6437,95 @@
         <v>C-20230628002</v>
       </c>
       <c r="C4" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="D4" s="33" t="s">
         <v>308</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>309</v>
-      </c>
       <c r="E4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="N4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="O4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="S4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="T4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="U4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="V4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="W4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="X4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Y4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Z4" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4C2CC8-3715-48D2-8986-FB374E83692E}">
-  <dimension ref="A1:Y2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4C2CC8-3715-48D2-8986-FB374E83692E}">
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
+    <sheetView topLeftCell="N1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="25.77734375" collapsed="true"/>
-    <col min="3" max="24" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="1" max="2" width="25.77734375" customWidth="1" collapsed="1"/>
+    <col min="3" max="24" width="15.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
@@ -6673,13 +6667,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C72F5EF2-9BE7-4D3D-81A0-9429E5F78E70}">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C72F5EF2-9BE7-4D3D-81A0-9429E5F78E70}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
@@ -6687,10 +6681,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.88671875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="3" max="7" customWidth="true" width="25.77734375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="36.33203125" collapsed="true"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="7" width="25.77734375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="36.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -6719,7 +6713,7 @@
         <v>238</v>
       </c>
     </row>
-    <row ht="57.6" r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="str">
         <f>'TC6-Supplier Contract Route'!A2</f>
         <v>scenario9001</v>
@@ -6746,7 +6740,7 @@
         <v>239</v>
       </c>
     </row>
-    <row ht="57.6" r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="str">
         <f>'TC6-Supplier Contract Route'!A3</f>
         <v>scenario9002</v>
@@ -6799,13 +6793,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7174A027-A196-42E5-B870-932CB2DA22DE}">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7174A027-A196-42E5-B870-932CB2DA22DE}">
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
@@ -6813,10 +6807,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.88671875" collapsed="true"/>
-    <col min="2" max="6" customWidth="true" width="25.77734375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="46.5546875" collapsed="true"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="6" width="25.77734375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="46.5546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -6845,18 +6839,18 @@
         <v>238</v>
       </c>
     </row>
-    <row ht="28.8" r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="str">
         <f>'TC6-Supplier Contract Route'!A2</f>
         <v>scenario9001</v>
       </c>
       <c r="B2" t="str">
         <f>'TC46-BU SO Delivery Plan (Date)'!A2</f>
-        <v>Nov 14, 2023</v>
+        <v>Nov 16, 2023</v>
       </c>
       <c r="C2" t="str">
         <f>'TC46-BU SO Delivery Plan (Date)'!B2</f>
-        <v>Nov 16, 2023</v>
+        <v>Nov 22, 2023</v>
       </c>
       <c r="D2" t="str">
         <f>'TC46-BU SO Delivery Plan (Date)'!C2</f>
@@ -6884,11 +6878,11 @@
       </c>
       <c r="B3" t="str">
         <f>'TC46-BU SO Delivery Plan (Date)'!A3</f>
-        <v>NULL</v>
+        <v>Nov 16, 2023</v>
       </c>
       <c r="C3" t="str">
         <f>'TC46-BU SO Delivery Plan (Date)'!B3</f>
-        <v>NULL</v>
+        <v>Nov 22, 2023</v>
       </c>
       <c r="D3" t="str">
         <f>'TC46-BU SO Delivery Plan (Date)'!C3</f>
@@ -6909,18 +6903,18 @@
         <v>244</v>
       </c>
     </row>
-    <row ht="28.8" r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="str">
         <f>'TC6-Supplier Contract Route'!A4</f>
         <v>scenario9003</v>
       </c>
       <c r="B4" t="str">
         <f>'TC46-BU SO Delivery Plan (Date)'!A4</f>
-        <v>NULL</v>
+        <v>Nov 16, 2023</v>
       </c>
       <c r="C4" t="str">
         <f>'TC46-BU SO Delivery Plan (Date)'!B4</f>
-        <v>NULL</v>
+        <v>Nov 22, 2023</v>
       </c>
       <c r="D4" t="str">
         <f>'TC46-BU SO Delivery Plan (Date)'!C4</f>
@@ -6943,13 +6937,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8A62EA-7F05-4B19-B65C-5B22C203BCD6}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8A62EA-7F05-4B19-B65C-5B22C203BCD6}">
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M40" sqref="M40"/>
@@ -6957,7 +6951,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="42.21875" collapsed="true"/>
+    <col min="1" max="1" width="42.21875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -6967,17 +6961,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9834B959-E77E-4B98-904B-D9A3CA9462D2}">
-  <dimension ref="A1:Z3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9834B959-E77E-4B98-904B-D9A3CA9462D2}">
+  <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Y1" sqref="Y1"/>
@@ -6985,84 +6979,84 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="25" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="1" max="25" width="15.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" ht="28.8" r="1" s="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>312</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>316</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>317</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I1" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>322</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>324</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>327</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>329</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>330</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>331</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>332</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>333</v>
-      </c>
-      <c r="Y1" s="7" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
@@ -7100,7 +7094,7 @@
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="O2" s="30">
         <v>1000</v>
@@ -7162,7 +7156,7 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="P3" s="30">
         <v>800</v>
@@ -7179,13 +7173,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C8279EE-7B75-4E84-A2EA-A5A57A2220BB}">
-  <dimension ref="A1:T3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C8279EE-7B75-4E84-A2EA-A5A57A2220BB}">
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -7193,66 +7187,66 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="19" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="1" max="19" width="15.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" ht="28.8" r="1" s="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>316</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>317</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="I1" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>322</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>324</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>326</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>327</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -7287,7 +7281,7 @@
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="O2" s="30">
         <v>1000</v>
@@ -7331,7 +7325,7 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="P3" s="30">
         <v>800</v>
@@ -7342,13 +7336,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD7DC5B-B487-4494-AD3C-76FDD10103AD}">
-  <dimension ref="A1:X4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD7DC5B-B487-4494-AD3C-76FDD10103AD}">
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
@@ -7356,78 +7350,78 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="23" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="1" max="23" width="15.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" ht="28.8" r="1" s="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>316</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>317</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="H1" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>318</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>319</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>322</v>
       </c>
-      <c r="M1" s="7" t="s">
-        <v>323</v>
-      </c>
       <c r="N1" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>337</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>339</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>340</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>341</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>342</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>343</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>344</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>345</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
@@ -7456,7 +7450,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N2" s="30">
         <v>500</v>
@@ -7502,7 +7496,7 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="O3" s="30"/>
       <c r="R3" s="30">
@@ -7538,7 +7532,7 @@
         <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="P4">
         <v>400</v>
@@ -7555,13 +7549,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E24C9F76-BC3D-4744-8035-BEC5FCCA69E6}">
-  <dimension ref="A1:Z2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E24C9F76-BC3D-4744-8035-BEC5FCCA69E6}">
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A41" sqref="A41"/>
@@ -7569,32 +7563,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="24.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.33203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.88671875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.88671875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.88671875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="15.21875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.6640625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="20.77734375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="17.88671875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="14.5546875" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="18.77734375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="16.77734375" collapsed="true"/>
-    <col min="26" max="16384" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="17" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="18.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="16384" width="8.88671875" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
@@ -7681,7 +7675,7 @@
       </c>
       <c r="B2" t="str">
         <f ca="1">TEXT(TODAY(),"dd MMM yyyy")</f>
-        <v>19 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
       <c r="D2">
         <v>1000</v>
@@ -7691,11 +7685,11 @@
       </c>
       <c r="F2" s="27" t="str">
         <f ca="1">TEXT(TODAY()+5,"dd MMM yyyy")</f>
-        <v>24 Oct 2023</v>
+        <v>06 Nov 2023</v>
       </c>
       <c r="G2" s="27" t="str">
         <f ca="1">TEXT(TODAY()+8,"dd MMM yyyy")</f>
-        <v>27 Oct 2023</v>
+        <v>09 Nov 2023</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>250</v>
@@ -7748,19 +7742,19 @@
       <c r="X2" s="28">
         <v>20.001000000000001</v>
       </c>
-      <c r="Y2" t="e">
+      <c r="Y2" t="str">
         <f ca="1">TEXT(G2, "mmm dd, yyyyy")</f>
-        <v>#VALUE!</v>
+        <v>Nov 09, 2023</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E6FAC1-DCE1-4444-890E-F6ABD609287F}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E6FAC1-DCE1-4444-890E-F6ABD609287F}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -7768,8 +7762,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.44140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -7786,17 +7780,17 @@
         <v>o-PK-SUP-POC-E-02-003</v>
       </c>
       <c r="B2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D5EB0F8-0C81-4EEF-9F42-0FAE32BB51CE}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D5EB0F8-0C81-4EEF-9F42-0FAE32BB51CE}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -7804,7 +7798,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="1" max="3" width="15.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -7852,13 +7846,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74284CB9-CE45-4423-874D-4BF43395C192}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74284CB9-CE45-4423-874D-4BF43395C192}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
@@ -7866,8 +7860,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.5546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="1" max="1" width="25.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -7884,7 +7878,7 @@
         <v>o-PK-SUP-POC-231012001</v>
       </c>
       <c r="B2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -7893,7 +7887,7 @@
         <v>o-PK-SUP-POC-231012002</v>
       </c>
       <c r="B3" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -7902,12 +7896,12 @@
         <v>o-PK-SUP-POC-231005003</v>
       </c>
       <c r="B4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C5" t="s">
         <v>248</v>
@@ -7915,13 +7909,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6561484A-194E-49A5-B09A-77F8C8B229C9}">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6561484A-194E-49A5-B09A-77F8C8B229C9}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
@@ -7929,8 +7923,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.77734375" collapsed="true"/>
-    <col min="2" max="15" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="1" max="1" width="25.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="15" width="15.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -8029,13 +8023,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CDA4C05-F9F8-45C6-A81B-365305D92F83}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CDA4C05-F9F8-45C6-A81B-365305D92F83}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
@@ -8043,8 +8037,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.44140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -8061,18 +8055,18 @@
         <v>o-PK-SUP-POC-231012002</v>
       </c>
       <c r="B2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A8511A-8D46-480D-B278-8DB3C522434C}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A8511A-8D46-480D-B278-8DB3C522434C}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A3"/>
@@ -8080,8 +8074,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="26.6640625" collapsed="true"/>
+    <col min="1" max="1" width="26.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -8123,13 +8117,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8558E625-8607-42E6-AA92-98E63C7FBFA1}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8558E625-8607-42E6-AA92-98E63C7FBFA1}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B3"/>
@@ -8137,8 +8131,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="38.88671875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="1" max="1" width="38.88671875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -8156,7 +8150,7 @@
       </c>
       <c r="B2" t="str">
         <f ca="1">TEXT(TODAY(),"dd MMM yyyy")</f>
-        <v>19 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -8166,7 +8160,7 @@
       </c>
       <c r="B3" t="str">
         <f ca="1">TEXT(TODAY(),"dd MMM yyyy")</f>
-        <v>19 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -8176,17 +8170,17 @@
       </c>
       <c r="B4" t="str">
         <f ca="1">TEXT(TODAY(),"dd MMM yyyy")</f>
-        <v>19 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFBFFFDE-1F89-4623-AC23-4DEDB73476D7}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFBFFFDE-1F89-4623-AC23-4DEDB73476D7}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -8194,7 +8188,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="1" max="3" width="15.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -8242,13 +8236,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD122CC-5234-4364-B477-E70360EB5335}">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD122CC-5234-4364-B477-E70360EB5335}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
@@ -8256,33 +8250,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="8" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="1" max="8" width="20.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" t="s">
         <v>278</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>279</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>280</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>281</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>282</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>283</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>284</v>
-      </c>
-      <c r="H1" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -8327,52 +8321,50 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B54E8F4-AAE1-4131-9CD0-7F416DDA1D91}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B54E8F4-AAE1-4131-9CD0-7F416DDA1D91}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" customWidth="true" width="20.77734375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="20.77734375" collapsed="true"/>
-    <col min="8" max="9" customWidth="true" width="20.77734375" collapsed="true"/>
+    <col min="1" max="9" width="20.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" t="s">
         <v>278</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>279</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>280</v>
       </c>
-      <c r="D1" t="s">
-        <v>281</v>
-      </c>
       <c r="E1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="G1" t="s">
         <v>13</v>
       </c>
       <c r="H1" t="s">
+        <v>283</v>
+      </c>
+      <c r="I1" t="s">
         <v>284</v>
-      </c>
-      <c r="I1" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -8405,46 +8397,46 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96C70245-C4A5-4550-B361-08466A958C3C}">
-  <dimension ref="A1:Z3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96C70245-C4A5-4550-B361-08466A958C3C}">
+  <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="24.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.33203125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.88671875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="13.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.88671875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="15.21875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.6640625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="19.21875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="20.88671875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="17.88671875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="8.77734375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="13.109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="18.88671875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="12.21875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="13.88671875" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="16.77734375" collapsed="true"/>
-    <col min="26" max="16384" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="17.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="8.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="17" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="18.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="12.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="13.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="16.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="16384" width="8.88671875" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
@@ -8531,7 +8523,7 @@
       </c>
       <c r="B2" t="str">
         <f ca="1">TEXT(TODAY(),"dd MMM yyyy")</f>
-        <v>19 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
       <c r="D2" s="31">
         <v>1200</v>
@@ -8541,11 +8533,11 @@
       </c>
       <c r="F2" s="27" t="str">
         <f ca="1">TEXT(TODAY()+5,"dd MMM yyyy")</f>
-        <v>24 Oct 2023</v>
+        <v>06 Nov 2023</v>
       </c>
       <c r="G2" s="27" t="str">
         <f ca="1">TEXT(TODAY()+8,"dd MMM yyyy")</f>
-        <v>27 Oct 2023</v>
+        <v>09 Nov 2023</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>250</v>
@@ -8598,9 +8590,9 @@
       <c r="X2" s="28">
         <v>20.001000000000001</v>
       </c>
-      <c r="Y2" t="e">
+      <c r="Y2" t="str">
         <f ca="1">TEXT(G2, "mmm dd, yyyyy")</f>
-        <v>#VALUE!</v>
+        <v>Nov 09, 2023</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
@@ -8610,7 +8602,7 @@
       </c>
       <c r="B3" t="str">
         <f ca="1">TEXT(TODAY(),"dd MMM yyyy")</f>
-        <v>19 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
       <c r="D3" s="31">
         <v>600</v>
@@ -8620,11 +8612,11 @@
       </c>
       <c r="F3" s="27" t="str">
         <f ca="1">TEXT(TODAY()+5,"dd MMM yyyy")</f>
-        <v>24 Oct 2023</v>
+        <v>06 Nov 2023</v>
       </c>
       <c r="G3" s="27" t="str">
         <f ca="1">TEXT(TODAY()+8,"dd MMM yyyy")</f>
-        <v>27 Oct 2023</v>
+        <v>09 Nov 2023</v>
       </c>
       <c r="H3" s="11" t="s">
         <v>260</v>
@@ -8667,13 +8659,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD33A310-6118-4E55-9BE2-B92D394BF9DA}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD33A310-6118-4E55-9BE2-B92D394BF9DA}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
@@ -8681,8 +8673,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.44140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -8699,17 +8691,17 @@
         <v>o-PK-CUS-DC-E-02-001</v>
       </c>
       <c r="B2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87B20617-E81D-4BA9-AE8A-69D2EA40FC8A}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87B20617-E81D-4BA9-AE8A-69D2EA40FC8A}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -8717,9 +8709,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="1" max="1" width="26.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -8736,7 +8728,7 @@
         <v>o-PK-SUP-POC-231012002</v>
       </c>
       <c r="B2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C2" t="s">
         <v>261</v>
@@ -8748,20 +8740,20 @@
         <v>o-PK-CUS-DC-231004002</v>
       </c>
       <c r="B3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C3" t="s">
         <v>262</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9FA60E-F1EA-41AC-BB7C-02445F118F92}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E9FA60E-F1EA-41AC-BB7C-02445F118F92}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -8769,8 +8761,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.21875" collapsed="true"/>
-    <col min="2" max="5" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="1" max="1" width="24.21875" customWidth="1" collapsed="1"/>
+    <col min="2" max="5" width="15.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -8797,7 +8789,7 @@
       </c>
       <c r="B2" t="str">
         <f ca="1">TEXT(TODAY(),"dd MMM yyyy")</f>
-        <v>19 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -8807,7 +8799,7 @@
       </c>
       <c r="B3" t="str">
         <f ca="1">TEXT(TODAY(),"dd MMM yyyy")</f>
-        <v>19 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -8817,7 +8809,7 @@
       </c>
       <c r="B4" t="str">
         <f ca="1">TEXT(TODAY(),"dd MMM yyyy")</f>
-        <v>19 Oct 2023</v>
+        <v>01 Nov 2023</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -8830,13 +8822,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88CDDF29-2529-4DC5-92A1-2CCBC9DFA340}">
-  <dimension ref="A1:W4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88CDDF29-2529-4DC5-92A1-2CCBC9DFA340}">
+  <dimension ref="A1:AD4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
@@ -8844,16 +8836,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="4.77734375" collapsed="true"/>
-    <col min="2" max="4" customWidth="true" width="20.77734375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="25.77734375" collapsed="true"/>
-    <col min="6" max="21" customWidth="true" width="15.77734375" collapsed="true"/>
-    <col min="22" max="22" width="8.88671875" collapsed="true"/>
-    <col min="24" max="24" width="8.88671875" collapsed="true"/>
-    <col min="31" max="16384" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="4.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="4" width="20.77734375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="25.77734375" customWidth="1" collapsed="1"/>
+    <col min="6" max="21" width="15.77734375" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="8.88671875" collapsed="1"/>
+    <col min="24" max="24" width="8.88671875" collapsed="1"/>
+    <col min="31" max="16384" width="8.88671875" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>27</v>
       </c>
@@ -9095,14 +9087,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085221D1-6E39-4DA5-AAB8-195C01175B25}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{085221D1-6E39-4DA5-AAB8-195C01175B25}">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -9110,8 +9102,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.44140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -9143,13 +9135,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD05878D-6B90-44F5-B8B4-C0B894310C69}">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD05878D-6B90-44F5-B8B4-C0B894310C69}">
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -9157,11 +9149,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.5546875" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="20.77734375" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" width="25.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="26.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="20.77734375" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="25.77734375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="26.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -9189,10 +9181,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C2" t="str">
         <f>B2&amp;"s"</f>
@@ -9265,28 +9257,28 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError formula="1" sqref="E3"/>
+    <ignoredError sqref="E3" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{223BB180-3190-4DAF-B2E7-03E84514429E}">
-  <dimension ref="A1:R2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{223BB180-3190-4DAF-B2E7-03E84514429E}">
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="4.77734375" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="25.77734375" collapsed="true"/>
-    <col min="4" max="16" customWidth="true" width="15.77734375" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="25.77734375" collapsed="true"/>
+    <col min="1" max="1" width="4.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="25.77734375" customWidth="1" collapsed="1"/>
+    <col min="4" max="16" width="15.77734375" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="25.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -9347,7 +9339,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C2" t="str">
         <f>"PKTTAP-PKCUS-"&amp;AutoIncrement!B2&amp;"-0"&amp;AutoIncrement!A2</f>
@@ -9396,17 +9388,17 @@
         <v>106</v>
       </c>
       <c r="Q2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E22683-5E59-4F52-830B-E9C218A1C72C}">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E22683-5E59-4F52-830B-E9C218A1C72C}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -9414,10 +9406,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" customWidth="true" width="25.77734375" collapsed="true"/>
+    <col min="1" max="7" width="25.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
@@ -9440,7 +9432,7 @@
         <v>39</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>138</v>
       </c>
@@ -9464,7 +9456,7 @@
         <v>78</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>139</v>
       </c>
@@ -9488,7 +9480,7 @@
         <v>78</v>
       </c>
     </row>
-    <row customFormat="1" r="4" s="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>140</v>
       </c>
@@ -9513,22 +9505,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E713B669-2ED0-4047-95AA-81FFB864CFE0}">
-  <dimension ref="A1:Y2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E713B669-2ED0-4047-95AA-81FFB864CFE0}">
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
+    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="25.77734375" collapsed="true"/>
-    <col min="3" max="24" customWidth="true" width="15.77734375" collapsed="true"/>
+    <col min="1" max="2" width="25.77734375" customWidth="1" collapsed="1"/>
+    <col min="3" max="24" width="15.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
@@ -9670,20 +9662,11 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010097067AA9A672F346A1B58BE42AD9877C" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fb25f0482db5a79c3d6b5c0926ca00a3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c3e097ef-e44a-4305-852f-ab2ffd6265ef" xmlns:ns3="1febb254-c9d7-4bcc-acc6-e4d894a01278" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="67b0f0bb964429d84d53f322277e62a8" ns2:_="" ns3:_="">
     <xsd:import namespace="c3e097ef-e44a-4305-852f-ab2ffd6265ef"/>
@@ -9854,15 +9837,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91ABF6FE-6484-4589-BC3D-47FF7C8B2779}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2F8FA2A-FCE7-4279-BCAB-0886BF9197B3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9879,4 +9863,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91ABF6FE-6484-4589-BC3D-47FF7C8B2779}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>